<commit_message>
- DONE: bug "late 1 min" is fixed
</commit_message>
<xml_diff>
--- a/Send it later/Tasks.xlsx
+++ b/Send it later/Tasks.xlsx
@@ -9,14 +9,14 @@
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
     <sheet name="Important rating" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Resolutions" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>Refactor the adapters</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>Database</t>
+  </si>
+  <si>
+    <t>Bug: Late 1 min</t>
   </si>
 </sst>
 </file>
@@ -140,12 +143,12 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -441,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -464,25 +467,25 @@
       <c r="C1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" s="2" customFormat="1">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -490,13 +493,13 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="D3">
         <v>3</v>
@@ -507,13 +510,13 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -522,42 +525,56 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="3" customFormat="1">
-      <c r="A5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" t="s">
+    <row r="5" spans="1:5" s="2" customFormat="1">
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="2">
         <v>2</v>
       </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
+      <c r="E5" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3" t="s">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="3">
-        <v>3</v>
-      </c>
-      <c r="E6" s="3">
+      <c r="D6" s="2">
+        <v>3</v>
+      </c>
+      <c r="E6" s="2">
         <v>1</v>
       </c>
     </row>
+    <row r="7" spans="1:5" s="2" customFormat="1">
+      <c r="A7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="2">
+        <v>3</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A2:E14">
-    <sortCondition ref="E2:E14"/>
-    <sortCondition ref="D2:D14"/>
+  <sortState ref="A2:E7">
+    <sortCondition ref="E2:E7"/>
+    <sortCondition ref="D2:D7"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -578,11 +595,11 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:4">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:4">
       <c r="A5">

</xml_diff>

<commit_message>
- Refactoring : adapters
</commit_message>
<xml_diff>
--- a/Send it later/Tasks.xlsx
+++ b/Send it later/Tasks.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
   <si>
     <t>Refactor the adapters</t>
   </si>
@@ -99,7 +99,25 @@
     <t>improvement</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t xml:space="preserve">On Click contacts list : ask before delete </t>
+  </si>
+  <si>
+    <t>EditMessage</t>
+  </si>
+  <si>
+    <t>Refactor the SentItem &amp; PendingItem : to MessageItem</t>
+  </si>
+  <si>
+    <t>Refactor SentAdapter &amp; PendingAdapter</t>
+  </si>
+  <si>
+    <t>IMessageList Is a interface - better than Common Super class</t>
+  </si>
+  <si>
+    <t>Wording: max_sent_item</t>
+  </si>
+  <si>
+    <t>String</t>
   </si>
 </sst>
 </file>
@@ -155,7 +173,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -167,6 +185,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,15 +480,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -605,12 +624,53 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
+    <row r="9" spans="1:5" s="6" customFormat="1" ht="18" customHeight="1">
+      <c r="A9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="6"/>
-    </row>
+      <c r="B9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="6">
+        <v>3</v>
+      </c>
+      <c r="E9" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="6" customFormat="1">
+      <c r="A10" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="6">
+        <v>2</v>
+      </c>
+      <c r="E10" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="6" customFormat="1"/>
+    <row r="12" spans="1:5" s="6" customFormat="1"/>
+    <row r="13" spans="1:5" s="6" customFormat="1"/>
+    <row r="14" spans="1:5" s="6" customFormat="1"/>
+    <row r="15" spans="1:5" s="6" customFormat="1"/>
+    <row r="16" spans="1:5" s="6" customFormat="1"/>
+    <row r="17" s="6" customFormat="1"/>
+    <row r="18" s="6" customFormat="1"/>
+    <row r="19" s="6" customFormat="1"/>
+    <row r="20" s="6" customFormat="1"/>
+    <row r="21" s="6" customFormat="1"/>
+    <row r="22" s="6" customFormat="1"/>
+    <row r="23" s="6" customFormat="1"/>
   </sheetData>
   <sortState ref="A2:E7">
     <sortCondition ref="E2:E7"/>
@@ -730,12 +790,45 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="6" customFormat="1">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- DONE: refactored 2 adapters
</commit_message>
<xml_diff>
--- a/Send it later/Tasks.xlsx
+++ b/Send it later/Tasks.xlsx
@@ -124,7 +124,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -136,6 +136,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -173,19 +179,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,7 +491,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A11" sqref="A11:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -512,47 +520,47 @@
     </row>
     <row r="2" spans="1:5" s="5" customFormat="1">
       <c r="A2" s="5" t="s">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="5">
         <v>2</v>
-      </c>
-      <c r="D2" s="5">
-        <v>3</v>
       </c>
       <c r="E2" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3">
-        <v>3</v>
-      </c>
-      <c r="E3">
+      <c r="A3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="4">
+        <v>3</v>
+      </c>
+      <c r="E3" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -561,120 +569,121 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="2" customFormat="1">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:5" s="5" customFormat="1">
+      <c r="A5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="5">
+        <v>3</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="5">
+        <v>3</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="5" customFormat="1">
+      <c r="A7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="5">
+        <v>3</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="5" customFormat="1">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D8" s="2">
         <v>2</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E8" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="2" t="s">
+    <row r="9" spans="1:5" s="5" customFormat="1" ht="18" customHeight="1">
+      <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2" t="s">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="2">
-        <v>3</v>
-      </c>
-      <c r="E6" s="2">
+      <c r="D9" s="2">
+        <v>3</v>
+      </c>
+      <c r="E9" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="2" customFormat="1">
-      <c r="A7" s="2" t="s">
+    <row r="10" spans="1:5" s="8" customFormat="1">
+      <c r="A10" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="B10" s="9"/>
+      <c r="C10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="2">
-        <v>3</v>
-      </c>
-      <c r="E7" s="2">
+      <c r="D10" s="9">
+        <v>3</v>
+      </c>
+      <c r="E10" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="6" customFormat="1">
-      <c r="A8" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="6">
-        <v>3</v>
-      </c>
-      <c r="E8" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" s="6" customFormat="1" ht="18" customHeight="1">
-      <c r="A9" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="6">
-        <v>3</v>
-      </c>
-      <c r="E9" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" s="6" customFormat="1">
-      <c r="A10" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="6">
-        <v>2</v>
-      </c>
-      <c r="E10" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" s="6" customFormat="1"/>
-    <row r="12" spans="1:5" s="6" customFormat="1"/>
-    <row r="13" spans="1:5" s="6" customFormat="1"/>
-    <row r="14" spans="1:5" s="6" customFormat="1"/>
-    <row r="15" spans="1:5" s="6" customFormat="1"/>
-    <row r="16" spans="1:5" s="6" customFormat="1"/>
-    <row r="17" s="6" customFormat="1"/>
-    <row r="18" s="6" customFormat="1"/>
-    <row r="19" s="6" customFormat="1"/>
-    <row r="20" s="6" customFormat="1"/>
-    <row r="21" s="6" customFormat="1"/>
-    <row r="22" s="6" customFormat="1"/>
-    <row r="23" s="6" customFormat="1"/>
+    <row r="11" spans="1:5" s="5" customFormat="1"/>
+    <row r="12" spans="1:5" s="5" customFormat="1"/>
+    <row r="13" spans="1:5" s="5" customFormat="1"/>
+    <row r="14" spans="1:5" s="5" customFormat="1"/>
+    <row r="15" spans="1:5" s="5" customFormat="1"/>
+    <row r="16" spans="1:5" s="5" customFormat="1"/>
+    <row r="17" s="5" customFormat="1"/>
+    <row r="18" s="5" customFormat="1"/>
+    <row r="19" s="5" customFormat="1"/>
+    <row r="20" s="5" customFormat="1"/>
+    <row r="21" s="5" customFormat="1"/>
+    <row r="22" s="5" customFormat="1"/>
+    <row r="23" s="5" customFormat="1"/>
   </sheetData>
-  <sortState ref="A2:E7">
-    <sortCondition ref="E2:E7"/>
-    <sortCondition ref="D2:D7"/>
+  <sortState ref="A2:E10">
+    <sortCondition ref="E2:E10"/>
+    <sortCondition ref="D2:D10"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -695,11 +704,11 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:4">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
     </row>
     <row r="5" spans="1:4">
       <c r="A5">
@@ -803,8 +812,8 @@
     <col min="3" max="3" width="55.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="6" customFormat="1">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:3" s="5" customFormat="1">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>